<commit_message>
excel files for ctc
</commit_message>
<xml_diff>
--- a/Green Line Info.xlsx
+++ b/Green Line Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{64DD429F-E320-45C6-AB13-F2972415AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63BE9B99-EF2E-4CE9-85EC-16B6AC98D6E3}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{64DD429F-E320-45C6-AB13-F2972415AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302F893A-C4A4-491C-AF41-5DBF03532908}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="11660" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="E149" sqref="E149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -582,303 +582,305 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D2" s="3">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3">
         <v>100</v>
       </c>
       <c r="D3" s="3">
-        <v>55</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3">
         <v>100</v>
       </c>
       <c r="D4" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D5" s="3">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D6" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3">
         <v>100</v>
       </c>
       <c r="D7" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3">
         <v>100</v>
       </c>
       <c r="D8" s="3">
-        <v>55</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
       </c>
       <c r="D10" s="3">
-        <v>55</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3">
         <v>100</v>
       </c>
       <c r="D11" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
       </c>
       <c r="D12" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>73</v>
       </c>
       <c r="C13" s="3">
         <v>100</v>
       </c>
       <c r="D13" s="3">
-        <v>55</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>74</v>
       </c>
       <c r="C14" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D14" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C15" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D15" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="4">
         <v>15</v>
       </c>
+      <c r="B16" s="3">
+        <v>76</v>
+      </c>
       <c r="C16" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D16" s="3">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="C17" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D17" s="3">
         <v>70</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C18" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D18" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D19" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C20" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D20" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="B21" s="3">
+        <v>81</v>
       </c>
       <c r="C21" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D21" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B22" s="4">
+        <v>82</v>
       </c>
       <c r="C22" s="3">
         <v>300</v>
@@ -889,10 +891,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="4">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="B23" s="3">
+        <v>83</v>
       </c>
       <c r="C23" s="3">
         <v>300</v>
@@ -900,16 +902,13 @@
       <c r="D23" s="3">
         <v>70</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="C24" s="3">
         <v>300</v>
@@ -920,10 +919,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3">
         <v>300</v>
@@ -934,561 +933,503 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B26" s="4">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D26" s="3">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="C27" s="3">
-        <v>100</v>
+        <v>86.6</v>
       </c>
       <c r="D27" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="4">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="B28" s="3">
+        <v>88</v>
       </c>
       <c r="C28" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B29" s="3">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B30" s="4">
+        <v>90</v>
       </c>
       <c r="C30" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D30" s="3">
-        <v>70</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="4">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="B31" s="3">
+        <v>91</v>
       </c>
       <c r="C31" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B32" s="3">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C32" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D32" s="3">
-        <v>70</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="4">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B33" s="3">
+        <v>93</v>
       </c>
       <c r="C33" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D33" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="3">
-        <v>33</v>
+        <v>18</v>
+      </c>
+      <c r="B34" s="4">
+        <v>94</v>
       </c>
       <c r="C34" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D34" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B35" s="3">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="C35" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="4">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B36" s="3">
+        <v>96</v>
       </c>
       <c r="C36" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D36" s="3">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B37" s="3">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="C37" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D37" s="3">
-        <v>70</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="3">
-        <v>37</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="4">
+        <v>98</v>
       </c>
       <c r="C38" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D38" s="3">
-        <v>70</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="4">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="B39" s="3">
+        <v>99</v>
       </c>
       <c r="C39" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D39" s="3">
-        <v>70</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B40" s="3">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="C40" s="3">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D40" s="3">
-        <v>70</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B41" s="3">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3">
-        <v>70</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B42" s="4">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="C42" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D42" s="3">
-        <v>70</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C43" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D43" s="3">
-        <v>70</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B44" s="3">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="C44" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D44" s="3">
-        <v>70</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="4">
-        <v>44</v>
+        <v>22</v>
+      </c>
+      <c r="B45" s="3">
+        <v>105</v>
       </c>
       <c r="C45" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D45" s="3">
-        <v>70</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+      <c r="E45" s="5" t="str">
+        <f>E13</f>
+        <v>STATION; DORMONT</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="3">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="B46" s="4">
+        <v>106</v>
       </c>
       <c r="C46" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D46" s="3">
-        <v>70</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B47" s="3">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C47" s="3">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D47" s="3">
-        <v>70</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="4">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="B48" s="3">
+        <v>108</v>
       </c>
       <c r="C48" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D48" s="3">
-        <v>70</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B49" s="3">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="C49" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D49" s="3">
-        <v>70</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="3">
-        <v>49</v>
+        <v>23</v>
+      </c>
+      <c r="B50" s="4">
+        <v>110</v>
       </c>
       <c r="C50" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D50" s="3">
         <v>70</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="4">
-        <v>50</v>
+        <v>23</v>
+      </c>
+      <c r="B51" s="3">
+        <v>111</v>
       </c>
       <c r="C51" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D51" s="3">
         <v>70</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B52" s="3">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="C52" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D52" s="3">
         <v>70</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B53" s="3">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C53" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D53" s="3">
         <v>70</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B54" s="4">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="C54" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D54" s="3">
         <v>70</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>34</v>
+      <c r="E54" s="5" t="str">
+        <f>E5</f>
+        <v>STATION; GLENBURY</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B55" s="3">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="C55" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D55" s="3">
         <v>70</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B56" s="3">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="C56" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D56" s="3">
         <v>70</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="4">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="B57" s="3">
+        <v>117</v>
       </c>
       <c r="C57" s="3">
         <v>50</v>
       </c>
       <c r="D57" s="3">
-        <v>70</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="3">
-        <v>57</v>
+        <v>24</v>
+      </c>
+      <c r="B58" s="4">
+        <v>118</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
       </c>
       <c r="D58" s="3">
-        <v>70</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B59" s="3">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="C59" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D59" s="3">
         <v>60</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="4">
-        <v>59</v>
+        <v>24</v>
+      </c>
+      <c r="B60" s="3">
+        <v>120</v>
       </c>
       <c r="C60" s="3">
         <v>50</v>
@@ -1499,10 +1440,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B61" s="3">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="C61" s="3">
         <v>50</v>
@@ -1513,440 +1454,489 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="3">
-        <v>61</v>
+        <v>25</v>
+      </c>
+      <c r="B62" s="4">
+        <v>122</v>
       </c>
       <c r="C62" s="3">
         <v>50</v>
       </c>
       <c r="D62" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="4">
-        <v>62</v>
+        <v>25</v>
+      </c>
+      <c r="B63" s="3">
+        <v>123</v>
       </c>
       <c r="C63" s="3">
         <v>50</v>
       </c>
       <c r="D63" s="3">
-        <v>60</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>39</v>
+        <v>70</v>
+      </c>
+      <c r="E63" s="5" t="str">
+        <f>E138</f>
+        <v>STATION; OVERBROOK; UNDERGROUND</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B64" s="3">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="C64" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D64" s="3">
         <v>70</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B65" s="3">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="C65" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D65" s="3">
         <v>70</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B66" s="4">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="C66" s="3">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D66" s="3">
         <v>70</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>40</v>
+      <c r="E66" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B67" s="3">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="C67" s="3">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D67" s="3">
         <v>70</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B68" s="3">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="C68" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D68" s="3">
         <v>70</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="4">
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="B69" s="3">
+        <v>129</v>
       </c>
       <c r="C69" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D69" s="3">
         <v>70</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" s="3">
-        <v>69</v>
+        <v>25</v>
+      </c>
+      <c r="B70" s="4">
+        <v>130</v>
       </c>
       <c r="C70" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D70" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B71" s="3">
-        <v>70</v>
+        <v>131</v>
       </c>
       <c r="C71" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D71" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72" s="4">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="B72" s="3">
+        <v>132</v>
       </c>
       <c r="C72" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D72" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E72" s="5" t="str">
+        <f>E129</f>
+        <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B73" s="3">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="C73" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D73" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="3">
-        <v>73</v>
+        <v>25</v>
+      </c>
+      <c r="B74" s="4">
+        <v>134</v>
       </c>
       <c r="C74" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D74" s="3">
-        <v>60</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B75" s="4">
-        <v>74</v>
+        <v>25</v>
+      </c>
+      <c r="B75" s="3">
+        <v>135</v>
       </c>
       <c r="C75" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D75" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B76" s="3">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="C76" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D76" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B77" s="3">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C77" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D77" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="3">
-        <v>77</v>
+        <v>25</v>
+      </c>
+      <c r="B78" s="4">
+        <v>138</v>
       </c>
       <c r="C78" s="3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D78" s="3">
         <v>70</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>42</v>
+      <c r="E78" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" s="4">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="B79" s="3">
+        <v>139</v>
       </c>
       <c r="C79" s="3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D79" s="3">
         <v>70</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B80" s="3">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="C80" s="3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D80" s="3">
         <v>70</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B81" s="3">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="C81" s="3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D81" s="3">
         <v>70</v>
+      </c>
+      <c r="E81" s="5" t="str">
+        <f>E120</f>
+        <v>STATION; CENTRAL; UNDERDROUND</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B82" s="3">
-        <v>81</v>
+        <v>3</v>
+      </c>
+      <c r="B82" s="4">
+        <v>1</v>
       </c>
       <c r="C82" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D82" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B83" s="4">
-        <v>82</v>
+        <v>3</v>
+      </c>
+      <c r="B83" s="3">
+        <v>2</v>
       </c>
       <c r="C83" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D83" s="3">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B84" s="3">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="C84" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D84" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B85" s="3">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="B85" s="4">
+        <v>4</v>
       </c>
       <c r="C85" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D85" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B86" s="3">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="C86" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D86" s="3">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B87" s="4">
-        <v>86</v>
+        <v>4</v>
+      </c>
+      <c r="B87" s="3">
+        <v>6</v>
       </c>
       <c r="C87" s="3">
         <v>100</v>
       </c>
       <c r="D87" s="3">
         <v>55</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" s="3">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="B88" s="4">
+        <v>7</v>
       </c>
       <c r="C88" s="3">
-        <v>86.6</v>
+        <v>100</v>
       </c>
       <c r="D88" s="3">
         <v>55</v>
       </c>
+      <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B89" s="3">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="C89" s="3">
         <v>100</v>
       </c>
       <c r="D89" s="3">
         <v>55</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B90" s="3">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="C90" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D90" s="3">
         <v>55</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B91" s="4">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C91" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D91" s="3">
         <v>55</v>
@@ -1954,13 +1944,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B92" s="3">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="C92" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D92" s="3">
         <v>55</v>
@@ -1968,272 +1958,277 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B93" s="3">
-        <v>92</v>
+        <v>5</v>
+      </c>
+      <c r="B93" s="4">
+        <v>12</v>
       </c>
       <c r="C93" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D93" s="3">
         <v>55</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B94" s="3">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="C94" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D94" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" s="4">
-        <v>94</v>
+        <v>6</v>
+      </c>
+      <c r="B95" s="3">
+        <v>14</v>
       </c>
       <c r="C95" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D95" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B96" s="3">
-        <v>95</v>
+        <v>6</v>
+      </c>
+      <c r="B96" s="4">
+        <v>15</v>
       </c>
       <c r="C96" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D96" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B97" s="3">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="C97" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D97" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B98" s="3">
-        <v>97</v>
+        <v>7</v>
+      </c>
+      <c r="B98" s="4">
+        <v>17</v>
       </c>
       <c r="C98" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D98" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B99" s="4">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="B99" s="3">
+        <v>18</v>
       </c>
       <c r="C99" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D99" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="3">
         <v>19</v>
       </c>
-      <c r="B100" s="3">
-        <v>99</v>
-      </c>
       <c r="C100" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D100" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B101" s="3">
-        <v>100</v>
+        <v>7</v>
+      </c>
+      <c r="B101" s="4">
+        <v>20</v>
       </c>
       <c r="C101" s="3">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D101" s="3">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B102" s="3">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="C102" s="3">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="D102" s="3">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B103" s="4">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="C103" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D103" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B104" s="3">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="C104" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D104" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B105" s="3">
-        <v>104</v>
+        <v>24</v>
       </c>
       <c r="C105" s="3">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="D105" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106" s="3">
-        <v>105</v>
+        <v>8</v>
+      </c>
+      <c r="B106" s="4">
+        <v>25</v>
       </c>
       <c r="C106" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D106" s="3">
-        <v>60</v>
-      </c>
-      <c r="E106" s="5" t="str">
-        <f>E74</f>
-        <v>STATION; DORMONT</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B107" s="4">
-        <v>106</v>
+        <v>8</v>
+      </c>
+      <c r="B107" s="3">
+        <v>26</v>
       </c>
       <c r="C107" s="3">
         <v>100</v>
       </c>
       <c r="D107" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B108" s="3">
-        <v>107</v>
+        <v>8</v>
+      </c>
+      <c r="B108" s="4">
+        <v>27</v>
       </c>
       <c r="C108" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="D108" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B109" s="3">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="C109" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D109" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B110" s="3">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="C110" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D110" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B111" s="4">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C111" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D111" s="3">
         <v>70</v>
@@ -2241,27 +2236,30 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B112" s="3">
-        <v>111</v>
+        <v>31</v>
       </c>
       <c r="C112" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D112" s="3">
         <v>70</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B113" s="3">
-        <v>112</v>
+        <v>9</v>
+      </c>
+      <c r="B113" s="4">
+        <v>32</v>
       </c>
       <c r="C113" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D113" s="3">
         <v>70</v>
@@ -2269,13 +2267,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B114" s="3">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="C114" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D114" s="3">
         <v>70</v>
@@ -2283,31 +2281,27 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B115" s="4">
-        <v>114</v>
+        <v>10</v>
+      </c>
+      <c r="B115" s="3">
+        <v>34</v>
       </c>
       <c r="C115" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D115" s="3">
         <v>70</v>
-      </c>
-      <c r="E115" s="5" t="str">
-        <f>E66</f>
-        <v>STATION; GLENBURY</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B116" s="3">
-        <v>115</v>
+        <v>10</v>
+      </c>
+      <c r="B116" s="4">
+        <v>35</v>
       </c>
       <c r="C116" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D116" s="3">
         <v>70</v>
@@ -2315,94 +2309,112 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B117" s="3">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="C117" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D117" s="3">
         <v>70</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B118" s="3">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="C118" s="3">
         <v>50</v>
       </c>
       <c r="D118" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B119" s="4">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C119" s="3">
         <v>50</v>
       </c>
       <c r="D119" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B120" s="3">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="C120" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D120" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B121" s="3">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="C121" s="3">
         <v>50</v>
       </c>
       <c r="D121" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B122" s="3">
-        <v>121</v>
+        <v>11</v>
+      </c>
+      <c r="B122" s="4">
+        <v>41</v>
       </c>
       <c r="C122" s="3">
         <v>50</v>
       </c>
       <c r="D122" s="3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B123" s="4">
-        <v>122</v>
+        <v>11</v>
+      </c>
+      <c r="B123" s="3">
+        <v>42</v>
       </c>
       <c r="C123" s="3">
         <v>50</v>
@@ -2416,10 +2428,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B124" s="3">
-        <v>123</v>
+        <v>43</v>
       </c>
       <c r="C124" s="3">
         <v>50</v>
@@ -2427,17 +2439,16 @@
       <c r="D124" s="3">
         <v>70</v>
       </c>
-      <c r="E124" s="5" t="str">
-        <f>E58</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
+      <c r="E124" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B125" s="3">
-        <v>124</v>
+        <v>11</v>
+      </c>
+      <c r="B125" s="4">
+        <v>44</v>
       </c>
       <c r="C125" s="3">
         <v>50</v>
@@ -2451,10 +2462,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B126" s="3">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="C126" s="3">
         <v>50</v>
@@ -2468,10 +2479,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B127" s="4">
-        <v>126</v>
+        <v>11</v>
+      </c>
+      <c r="B127" s="3">
+        <v>46</v>
       </c>
       <c r="C127" s="3">
         <v>50</v>
@@ -2485,10 +2496,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B128" s="3">
-        <v>127</v>
+        <v>11</v>
+      </c>
+      <c r="B128" s="4">
+        <v>47</v>
       </c>
       <c r="C128" s="3">
         <v>50</v>
@@ -2502,10 +2513,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B129" s="3">
-        <v>128</v>
+        <v>48</v>
       </c>
       <c r="C129" s="3">
         <v>50</v>
@@ -2513,16 +2524,16 @@
       <c r="D129" s="3">
         <v>70</v>
       </c>
-      <c r="E129" s="3" t="s">
-        <v>34</v>
+      <c r="E129" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B130" s="3">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="C130" s="3">
         <v>50</v>
@@ -2536,10 +2547,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B131" s="4">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="C131" s="3">
         <v>50</v>
@@ -2553,10 +2564,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B132" s="3">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="C132" s="3">
         <v>50</v>
@@ -2570,10 +2581,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B133" s="3">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C133" s="3">
         <v>50</v>
@@ -2581,17 +2592,16 @@
       <c r="D133" s="3">
         <v>70</v>
       </c>
-      <c r="E133" s="5" t="str">
-        <f>E49</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      <c r="E133" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B134" s="3">
-        <v>133</v>
+        <v>11</v>
+      </c>
+      <c r="B134" s="4">
+        <v>53</v>
       </c>
       <c r="C134" s="3">
         <v>50</v>
@@ -2605,10 +2615,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B135" s="4">
-        <v>134</v>
+        <v>11</v>
+      </c>
+      <c r="B135" s="3">
+        <v>54</v>
       </c>
       <c r="C135" s="3">
         <v>50</v>
@@ -2622,10 +2632,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B136" s="3">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="C136" s="3">
         <v>50</v>
@@ -2639,10 +2649,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B137" s="3">
-        <v>136</v>
+        <v>11</v>
+      </c>
+      <c r="B137" s="4">
+        <v>56</v>
       </c>
       <c r="C137" s="3">
         <v>50</v>
@@ -2656,10 +2666,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B138" s="3">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="C138" s="3">
         <v>50</v>
@@ -2667,77 +2677,67 @@
       <c r="D138" s="3">
         <v>70</v>
       </c>
-      <c r="E138" s="3" t="s">
-        <v>34</v>
+      <c r="E138" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B139" s="4">
-        <v>138</v>
+        <v>12</v>
+      </c>
+      <c r="B139" s="3">
+        <v>58</v>
       </c>
       <c r="C139" s="3">
         <v>50</v>
       </c>
       <c r="D139" s="3">
-        <v>70</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B140" s="3">
-        <v>139</v>
+        <v>12</v>
+      </c>
+      <c r="B140" s="4">
+        <v>59</v>
       </c>
       <c r="C140" s="3">
         <v>50</v>
       </c>
       <c r="D140" s="3">
-        <v>70</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B141" s="3">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C141" s="3">
         <v>50</v>
       </c>
       <c r="D141" s="3">
-        <v>70</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B142" s="3">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="C142" s="3">
         <v>50</v>
       </c>
       <c r="D142" s="3">
-        <v>70</v>
-      </c>
-      <c r="E142" s="5" t="str">
-        <f>E40</f>
-        <v>STATION; CENTRAL; UNDERDROUND</v>
+        <v>60</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ITERATION 3 BITCHES MUAHAHAHAHHAHAHAHA
</commit_message>
<xml_diff>
--- a/Green Line Info.xlsx
+++ b/Green Line Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\1140-Integration-SWTrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{64DD429F-E320-45C6-AB13-F2972415AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302F893A-C4A4-491C-AF41-5DBF03532908}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433871E-5900-4E6C-AC7C-0FDC92A164C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="46">
   <si>
     <t>Section</t>
   </si>
@@ -143,9 +143,6 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; CENTRAL; UNDERDROUND</t>
-  </si>
-  <si>
     <t>STATION; INGLEWOOD; UNDERGROUND</t>
   </si>
   <si>
@@ -171,6 +168,12 @@
   </si>
   <si>
     <t>STATION;   CASTLE SHANNON</t>
+  </si>
+  <si>
+    <t>STATION; CENTRAL; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -552,18 +555,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,43 +583,43 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5">
+        <v>151</v>
+      </c>
+      <c r="C2" s="5">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>62</v>
       </c>
-      <c r="C2" s="3">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3">
-        <v>60</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3">
-        <v>63</v>
-      </c>
       <c r="C3" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3">
         <v>100</v>
@@ -625,29 +628,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
-        <v>65</v>
+      <c r="B5" s="3">
+        <v>64</v>
       </c>
       <c r="C5" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3">
         <v>70</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3">
-        <v>66</v>
+      <c r="B6" s="4">
+        <v>65</v>
       </c>
       <c r="C6" s="3">
         <v>200</v>
@@ -655,55 +655,58 @@
       <c r="D6" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D7" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
         <v>68</v>
       </c>
-      <c r="C8" s="3">
-        <v>100</v>
-      </c>
-      <c r="D8" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>69</v>
-      </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
@@ -712,12 +715,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
-        <v>71</v>
+      <c r="B11" s="3">
+        <v>70</v>
       </c>
       <c r="C11" s="3">
         <v>100</v>
@@ -726,12 +729,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
-        <v>72</v>
+      <c r="B12" s="4">
+        <v>71</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
@@ -740,43 +743,43 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3">
+        <v>72</v>
+      </c>
+      <c r="C13" s="3">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
         <v>73</v>
       </c>
-      <c r="C13" s="3">
-        <v>100</v>
-      </c>
-      <c r="D13" s="3">
-        <v>60</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <v>74</v>
-      </c>
       <c r="C14" s="3">
         <v>100</v>
       </c>
       <c r="D14" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3">
-        <v>75</v>
+      <c r="B15" s="4">
+        <v>74</v>
       </c>
       <c r="C15" s="3">
         <v>100</v>
@@ -785,46 +788,43 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
         <v>76</v>
       </c>
-      <c r="C16" s="3">
-        <v>100</v>
-      </c>
-      <c r="D16" s="3">
-        <v>60</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C17" s="3">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <v>60</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <v>77</v>
-      </c>
-      <c r="C17" s="3">
-        <v>300</v>
-      </c>
-      <c r="D17" s="3">
-        <v>70</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <v>78</v>
+      <c r="B18" s="3">
+        <v>77</v>
       </c>
       <c r="C18" s="3">
         <v>300</v>
@@ -832,13 +832,16 @@
       <c r="D18" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3">
-        <v>79</v>
+      <c r="B19" s="4">
+        <v>78</v>
       </c>
       <c r="C19" s="3">
         <v>300</v>
@@ -847,12 +850,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3">
         <v>300</v>
@@ -861,12 +864,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3">
         <v>300</v>
@@ -875,12 +878,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4">
-        <v>82</v>
+      <c r="B22" s="3">
+        <v>81</v>
       </c>
       <c r="C22" s="3">
         <v>300</v>
@@ -889,12 +892,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="3">
-        <v>83</v>
+      <c r="B23" s="4">
+        <v>82</v>
       </c>
       <c r="C23" s="3">
         <v>300</v>
@@ -903,12 +906,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3">
         <v>300</v>
@@ -917,12 +920,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="3">
         <v>300</v>
@@ -931,74 +934,74 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="4">
-        <v>86</v>
+        <v>16</v>
+      </c>
+      <c r="B26" s="3">
+        <v>85</v>
       </c>
       <c r="C26" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D26" s="3">
-        <v>55</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="3">
-        <v>87</v>
+      <c r="B27" s="4">
+        <v>86</v>
       </c>
       <c r="C27" s="3">
-        <v>86.6</v>
+        <v>100</v>
       </c>
       <c r="D27" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="3">
+        <v>87</v>
+      </c>
+      <c r="C28" s="3">
+        <v>86.6</v>
+      </c>
+      <c r="D28" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
         <v>88</v>
       </c>
-      <c r="C28" s="3">
-        <v>100</v>
-      </c>
-      <c r="D28" s="3">
-        <v>55</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="3">
-        <v>89</v>
-      </c>
       <c r="C29" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D29" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4">
-        <v>90</v>
+      <c r="B30" s="3">
+        <v>89</v>
       </c>
       <c r="C30" s="3">
         <v>75</v>
@@ -1007,12 +1010,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="3">
-        <v>91</v>
+      <c r="B31" s="4">
+        <v>90</v>
       </c>
       <c r="C31" s="3">
         <v>75</v>
@@ -1021,12 +1024,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="3">
         <v>75</v>
@@ -1035,12 +1038,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3">
         <v>75</v>
@@ -1049,12 +1052,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="4">
-        <v>94</v>
+      <c r="B34" s="3">
+        <v>93</v>
       </c>
       <c r="C34" s="3">
         <v>75</v>
@@ -1063,12 +1066,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="3">
-        <v>95</v>
+      <c r="B35" s="4">
+        <v>94</v>
       </c>
       <c r="C35" s="3">
         <v>75</v>
@@ -1077,12 +1080,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="3">
         <v>75</v>
@@ -1090,16 +1093,13 @@
       <c r="D36" s="3">
         <v>55</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="3">
         <v>75</v>
@@ -1107,13 +1107,16 @@
       <c r="D37" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="4">
-        <v>98</v>
+        <v>18</v>
+      </c>
+      <c r="B38" s="3">
+        <v>97</v>
       </c>
       <c r="C38" s="3">
         <v>75</v>
@@ -1122,12 +1125,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="3">
-        <v>99</v>
+      <c r="B39" s="4">
+        <v>98</v>
       </c>
       <c r="C39" s="3">
         <v>75</v>
@@ -1136,12 +1139,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="3">
         <v>75</v>
@@ -1150,40 +1153,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="3">
+        <v>100</v>
+      </c>
+      <c r="C41" s="3">
+        <v>75</v>
+      </c>
+      <c r="D41" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="3">
         <v>101</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C42" s="3">
         <v>15</v>
       </c>
-      <c r="D41" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="4">
-        <v>102</v>
-      </c>
-      <c r="C42" s="3">
-        <v>100</v>
-      </c>
       <c r="D42" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="3">
-        <v>103</v>
+      <c r="B43" s="4">
+        <v>102</v>
       </c>
       <c r="C43" s="3">
         <v>100</v>
@@ -1192,44 +1195,40 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="3">
+        <v>103</v>
+      </c>
+      <c r="C44" s="3">
+        <v>100</v>
+      </c>
+      <c r="D44" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="3">
         <v>104</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C45" s="3">
         <v>80</v>
       </c>
-      <c r="D44" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="3">
-        <v>105</v>
-      </c>
-      <c r="C45" s="3">
-        <v>100</v>
-      </c>
       <c r="D45" s="3">
         <v>60</v>
       </c>
-      <c r="E45" s="5" t="str">
-        <f>E13</f>
-        <v>STATION; DORMONT</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="4">
-        <v>106</v>
+      <c r="B46" s="3">
+        <v>105</v>
       </c>
       <c r="C46" s="3">
         <v>100</v>
@@ -1237,69 +1236,73 @@
       <c r="D46" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="5" t="str">
+        <f>E14</f>
+        <v>STATION; DORMONT</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="3">
-        <v>107</v>
+      <c r="B47" s="4">
+        <v>106</v>
       </c>
       <c r="C47" s="3">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D47" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="3">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C48" s="3">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D48" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="3">
+        <v>108</v>
+      </c>
+      <c r="C49" s="3">
+        <v>100</v>
+      </c>
+      <c r="D49" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="3">
         <v>109</v>
       </c>
-      <c r="C49" s="3">
-        <v>100</v>
-      </c>
-      <c r="D49" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="4">
-        <v>110</v>
-      </c>
       <c r="C50" s="3">
         <v>100</v>
       </c>
       <c r="D50" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="3">
-        <v>111</v>
+      <c r="B51" s="4">
+        <v>110</v>
       </c>
       <c r="C51" s="3">
         <v>100</v>
@@ -1308,12 +1311,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" s="3">
         <v>100</v>
@@ -1322,12 +1325,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="3">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C53" s="3">
         <v>100</v>
@@ -1336,12 +1339,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="4">
-        <v>114</v>
+      <c r="B54" s="3">
+        <v>113</v>
       </c>
       <c r="C54" s="3">
         <v>100</v>
@@ -1349,17 +1352,13 @@
       <c r="D54" s="3">
         <v>70</v>
       </c>
-      <c r="E54" s="5" t="str">
-        <f>E5</f>
-        <v>STATION; GLENBURY</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="3">
-        <v>115</v>
+      <c r="B55" s="4">
+        <v>114</v>
       </c>
       <c r="C55" s="3">
         <v>100</v>
@@ -1367,41 +1366,45 @@
       <c r="D55" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E55" s="5" t="str">
+        <f>E6</f>
+        <v>STATION; GLENBURY</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="3">
+        <v>115</v>
+      </c>
+      <c r="C56" s="3">
+        <v>100</v>
+      </c>
+      <c r="D56" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="3">
         <v>116</v>
       </c>
-      <c r="C56" s="3">
-        <v>100</v>
-      </c>
-      <c r="D56" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="3">
-        <v>117</v>
-      </c>
       <c r="C57" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D57" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="4">
-        <v>118</v>
+      <c r="B58" s="3">
+        <v>117</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
@@ -1410,71 +1413,68 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="3">
-        <v>119</v>
+      <c r="B59" s="4">
+        <v>118</v>
       </c>
       <c r="C59" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D59" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="3">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C60" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D60" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="3">
+        <v>120</v>
+      </c>
+      <c r="C61" s="3">
+        <v>50</v>
+      </c>
+      <c r="D61" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="3">
         <v>121</v>
       </c>
-      <c r="C61" s="3">
-        <v>50</v>
-      </c>
-      <c r="D61" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="4">
-        <v>122</v>
-      </c>
       <c r="C62" s="3">
         <v>50</v>
       </c>
       <c r="D62" s="3">
-        <v>70</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="3">
-        <v>123</v>
+      <c r="B63" s="4">
+        <v>122</v>
       </c>
       <c r="C63" s="3">
         <v>50</v>
@@ -1482,17 +1482,16 @@
       <c r="D63" s="3">
         <v>70</v>
       </c>
-      <c r="E63" s="5" t="str">
-        <f>E138</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E63" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B64" s="3">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" s="3">
         <v>50</v>
@@ -1500,16 +1499,17 @@
       <c r="D64" s="3">
         <v>70</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E64" s="5" t="str">
+        <f>E139</f>
+        <v>STATION; OVERBROOK; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="3">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="3">
         <v>50</v>
@@ -1521,12 +1521,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="4">
-        <v>126</v>
+      <c r="B66" s="3">
+        <v>125</v>
       </c>
       <c r="C66" s="3">
         <v>50</v>
@@ -1538,12 +1538,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="3">
-        <v>127</v>
+      <c r="B67" s="4">
+        <v>126</v>
       </c>
       <c r="C67" s="3">
         <v>50</v>
@@ -1555,12 +1555,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="3">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C68" s="3">
         <v>50</v>
@@ -1572,12 +1572,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B69" s="3">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C69" s="3">
         <v>50</v>
@@ -1589,12 +1589,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="4">
-        <v>130</v>
+      <c r="B70" s="3">
+        <v>129</v>
       </c>
       <c r="C70" s="3">
         <v>50</v>
@@ -1606,12 +1606,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B71" s="3">
-        <v>131</v>
+      <c r="B71" s="4">
+        <v>130</v>
       </c>
       <c r="C71" s="3">
         <v>50</v>
@@ -1623,12 +1623,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="3">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C72" s="3">
         <v>50</v>
@@ -1636,17 +1636,16 @@
       <c r="D72" s="3">
         <v>70</v>
       </c>
-      <c r="E72" s="5" t="str">
-        <f>E129</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E72" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C73" s="3">
         <v>50</v>
@@ -1654,16 +1653,17 @@
       <c r="D73" s="3">
         <v>70</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E73" s="5" t="str">
+        <f>E130</f>
+        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" s="4">
-        <v>134</v>
+      <c r="B74" s="3">
+        <v>133</v>
       </c>
       <c r="C74" s="3">
         <v>50</v>
@@ -1675,12 +1675,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="3">
-        <v>135</v>
+      <c r="B75" s="4">
+        <v>134</v>
       </c>
       <c r="C75" s="3">
         <v>50</v>
@@ -1692,12 +1692,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B76" s="3">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C76" s="3">
         <v>50</v>
@@ -1709,12 +1709,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B77" s="3">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C77" s="3">
         <v>50</v>
@@ -1726,12 +1726,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="4">
-        <v>138</v>
+      <c r="B78" s="3">
+        <v>137</v>
       </c>
       <c r="C78" s="3">
         <v>50</v>
@@ -1743,12 +1743,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="3">
-        <v>139</v>
+      <c r="B79" s="4">
+        <v>138</v>
       </c>
       <c r="C79" s="3">
         <v>50</v>
@@ -1760,12 +1760,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B80" s="3">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C80" s="3">
         <v>50</v>
@@ -1777,44 +1777,47 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B81" s="3">
+        <v>140</v>
+      </c>
+      <c r="C81" s="3">
+        <v>50</v>
+      </c>
+      <c r="D81" s="3">
+        <v>70</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="3">
         <v>141</v>
       </c>
-      <c r="C81" s="3">
-        <v>50</v>
-      </c>
-      <c r="D81" s="3">
-        <v>70</v>
-      </c>
-      <c r="E81" s="5" t="str">
-        <f>E120</f>
-        <v>STATION; CENTRAL; UNDERDROUND</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="4">
-        <v>1</v>
-      </c>
       <c r="C82" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D82" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="E82" s="5" t="str">
+        <f>E121</f>
+        <v>STATION; CENTRAL; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="3">
-        <v>2</v>
+      <c r="B83" s="4">
+        <v>1</v>
       </c>
       <c r="C83" s="3">
         <v>100</v>
@@ -1822,30 +1825,30 @@
       <c r="D83" s="3">
         <v>55</v>
       </c>
-      <c r="E83" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="3">
+        <v>2</v>
+      </c>
+      <c r="C84" s="3">
+        <v>100</v>
+      </c>
+      <c r="D84" s="3">
+        <v>55</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="3">
-        <v>100</v>
-      </c>
-      <c r="D84" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="4">
-        <v>4</v>
+      <c r="B85" s="3">
+        <v>3</v>
       </c>
       <c r="C85" s="3">
         <v>100</v>
@@ -1854,12 +1857,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="3">
-        <v>5</v>
+      <c r="B86" s="4">
+        <v>4</v>
       </c>
       <c r="C86" s="3">
         <v>100</v>
@@ -1868,41 +1871,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="3">
+        <v>5</v>
+      </c>
+      <c r="C87" s="3">
+        <v>100</v>
+      </c>
+      <c r="D87" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="3">
         <v>6</v>
       </c>
-      <c r="C87" s="3">
-        <v>100</v>
-      </c>
-      <c r="D87" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="4">
-        <v>7</v>
-      </c>
       <c r="C88" s="3">
         <v>100</v>
       </c>
       <c r="D88" s="3">
         <v>55</v>
       </c>
-      <c r="E88" s="5"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="3">
-        <v>8</v>
+      <c r="B89" s="4">
+        <v>7</v>
       </c>
       <c r="C89" s="3">
         <v>100</v>
@@ -1910,13 +1912,14 @@
       <c r="D89" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B90" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90" s="3">
         <v>100</v>
@@ -1924,16 +1927,13 @@
       <c r="D90" s="3">
         <v>55</v>
       </c>
-      <c r="E90" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="4">
-        <v>10</v>
+      <c r="B91" s="3">
+        <v>9</v>
       </c>
       <c r="C91" s="3">
         <v>100</v>
@@ -1941,13 +1941,16 @@
       <c r="D91" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E91" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="3">
-        <v>11</v>
+      <c r="B92" s="4">
+        <v>10</v>
       </c>
       <c r="C92" s="3">
         <v>100</v>
@@ -1956,43 +1959,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93" s="3">
+        <v>11</v>
+      </c>
+      <c r="C93" s="3">
+        <v>100</v>
+      </c>
+      <c r="D93" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="4">
         <v>12</v>
       </c>
-      <c r="C93" s="3">
-        <v>100</v>
-      </c>
-      <c r="D93" s="3">
-        <v>55</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="C94" s="3">
+        <v>100</v>
+      </c>
+      <c r="D94" s="3">
+        <v>55</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="3">
-        <v>13</v>
-      </c>
-      <c r="C94" s="3">
-        <v>150</v>
-      </c>
-      <c r="D94" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95" s="3">
         <v>150</v>
@@ -2001,12 +2004,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="4">
-        <v>15</v>
+      <c r="B96" s="3">
+        <v>14</v>
       </c>
       <c r="C96" s="3">
         <v>150</v>
@@ -2015,12 +2018,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="3">
-        <v>16</v>
+      <c r="B97" s="4">
+        <v>15</v>
       </c>
       <c r="C97" s="3">
         <v>150</v>
@@ -2028,30 +2031,30 @@
       <c r="D97" s="3">
         <v>70</v>
       </c>
-      <c r="E97" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="4">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="B98" s="3">
+        <v>16</v>
       </c>
       <c r="C98" s="3">
         <v>150</v>
       </c>
       <c r="D98" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B99" s="3">
-        <v>18</v>
+      <c r="B99" s="4">
+        <v>17</v>
       </c>
       <c r="C99" s="3">
         <v>150</v>
@@ -2060,12 +2063,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C100" s="3">
         <v>150</v>
@@ -2074,12 +2077,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="4">
-        <v>20</v>
+      <c r="B101" s="3">
+        <v>19</v>
       </c>
       <c r="C101" s="3">
         <v>150</v>
@@ -2088,26 +2091,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" s="3">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="B102" s="4">
+        <v>20</v>
       </c>
       <c r="C102" s="3">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D102" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="4">
-        <v>22</v>
+      <c r="B103" s="3">
+        <v>21</v>
       </c>
       <c r="C103" s="3">
         <v>300</v>
@@ -2115,16 +2118,13 @@
       <c r="D103" s="3">
         <v>70</v>
       </c>
-      <c r="E103" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="3">
-        <v>23</v>
+      <c r="B104" s="4">
+        <v>22</v>
       </c>
       <c r="C104" s="3">
         <v>300</v>
@@ -2132,13 +2132,16 @@
       <c r="D104" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E104" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C105" s="3">
         <v>300</v>
@@ -2147,99 +2150,99 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="4">
-        <v>25</v>
+      <c r="B106" s="3">
+        <v>24</v>
       </c>
       <c r="C106" s="3">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D106" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="3">
-        <v>26</v>
+      <c r="B107" s="4">
+        <v>25</v>
       </c>
       <c r="C107" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D107" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="4">
-        <v>27</v>
+      <c r="B108" s="3">
+        <v>26</v>
       </c>
       <c r="C108" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D108" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="4">
+        <v>27</v>
+      </c>
+      <c r="C109" s="3">
+        <v>50</v>
+      </c>
+      <c r="D109" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="3">
         <v>28</v>
       </c>
-      <c r="C109" s="3">
-        <v>50</v>
-      </c>
-      <c r="D109" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110" s="3">
-        <v>29</v>
-      </c>
       <c r="C110" s="3">
         <v>50</v>
       </c>
       <c r="D110" s="3">
         <v>70</v>
       </c>
-      <c r="E110" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B111" s="4">
+      <c r="B111" s="3">
+        <v>29</v>
+      </c>
+      <c r="C111" s="3">
+        <v>50</v>
+      </c>
+      <c r="D111" s="3">
+        <v>70</v>
+      </c>
+      <c r="E111" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="3">
-        <v>50</v>
-      </c>
-      <c r="D111" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B112" s="3">
-        <v>31</v>
+      <c r="B112" s="4">
+        <v>30</v>
       </c>
       <c r="C112" s="3">
         <v>50</v>
@@ -2247,31 +2250,31 @@
       <c r="D112" s="3">
         <v>70</v>
       </c>
-      <c r="E112" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B113" s="3">
+        <v>31</v>
+      </c>
+      <c r="C113" s="3">
+        <v>50</v>
+      </c>
+      <c r="D113" s="3">
+        <v>70</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" s="4">
         <v>32</v>
       </c>
-      <c r="C113" s="3">
-        <v>50</v>
-      </c>
-      <c r="D113" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B114" s="3">
-        <v>33</v>
-      </c>
       <c r="C114" s="3">
         <v>50</v>
       </c>
@@ -2279,12 +2282,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B115" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C115" s="3">
         <v>50</v>
@@ -2293,43 +2296,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="4">
+      <c r="B116" s="3">
+        <v>34</v>
+      </c>
+      <c r="C116" s="3">
+        <v>50</v>
+      </c>
+      <c r="D116" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="4">
         <v>35</v>
       </c>
-      <c r="C116" s="3">
-        <v>50</v>
-      </c>
-      <c r="D116" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B117" s="3">
-        <v>36</v>
-      </c>
       <c r="C117" s="3">
         <v>50</v>
       </c>
       <c r="D117" s="3">
         <v>70</v>
       </c>
-      <c r="E117" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B118" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C118" s="3">
         <v>50</v>
@@ -2341,12 +2341,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="4">
-        <v>38</v>
+      <c r="B119" s="3">
+        <v>37</v>
       </c>
       <c r="C119" s="3">
         <v>50</v>
@@ -2358,12 +2358,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="3">
-        <v>39</v>
+      <c r="B120" s="4">
+        <v>38</v>
       </c>
       <c r="C120" s="3">
         <v>50</v>
@@ -2371,16 +2371,16 @@
       <c r="D120" s="3">
         <v>70</v>
       </c>
-      <c r="E120" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E120" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B121" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C121" s="3">
         <v>50</v>
@@ -2388,16 +2388,16 @@
       <c r="D121" s="3">
         <v>70</v>
       </c>
-      <c r="E121" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E121" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="4">
-        <v>41</v>
+      <c r="B122" s="3">
+        <v>40</v>
       </c>
       <c r="C122" s="3">
         <v>50</v>
@@ -2409,12 +2409,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="3">
-        <v>42</v>
+      <c r="B123" s="4">
+        <v>41</v>
       </c>
       <c r="C123" s="3">
         <v>50</v>
@@ -2426,12 +2426,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B124" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C124" s="3">
         <v>50</v>
@@ -2443,12 +2443,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="4">
-        <v>44</v>
+      <c r="B125" s="3">
+        <v>43</v>
       </c>
       <c r="C125" s="3">
         <v>50</v>
@@ -2460,12 +2460,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="3">
-        <v>45</v>
+      <c r="B126" s="4">
+        <v>44</v>
       </c>
       <c r="C126" s="3">
         <v>50</v>
@@ -2477,12 +2477,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B127" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C127" s="3">
         <v>50</v>
@@ -2494,12 +2494,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="4">
-        <v>47</v>
+      <c r="B128" s="3">
+        <v>46</v>
       </c>
       <c r="C128" s="3">
         <v>50</v>
@@ -2511,12 +2511,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="3">
-        <v>48</v>
+      <c r="B129" s="4">
+        <v>47</v>
       </c>
       <c r="C129" s="3">
         <v>50</v>
@@ -2524,16 +2524,16 @@
       <c r="D129" s="3">
         <v>70</v>
       </c>
-      <c r="E129" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E129" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B130" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C130" s="3">
         <v>50</v>
@@ -2541,16 +2541,16 @@
       <c r="D130" s="3">
         <v>70</v>
       </c>
-      <c r="E130" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E130" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="4">
-        <v>50</v>
+      <c r="B131" s="3">
+        <v>49</v>
       </c>
       <c r="C131" s="3">
         <v>50</v>
@@ -2562,12 +2562,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="3">
-        <v>51</v>
+      <c r="B132" s="4">
+        <v>50</v>
       </c>
       <c r="C132" s="3">
         <v>50</v>
@@ -2579,12 +2579,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B133" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C133" s="3">
         <v>50</v>
@@ -2596,12 +2596,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B134" s="4">
-        <v>53</v>
+      <c r="B134" s="3">
+        <v>52</v>
       </c>
       <c r="C134" s="3">
         <v>50</v>
@@ -2613,12 +2613,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B135" s="3">
-        <v>54</v>
+      <c r="B135" s="4">
+        <v>53</v>
       </c>
       <c r="C135" s="3">
         <v>50</v>
@@ -2630,12 +2630,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B136" s="3">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C136" s="3">
         <v>50</v>
@@ -2647,12 +2647,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B137" s="4">
-        <v>56</v>
+      <c r="B137" s="3">
+        <v>55</v>
       </c>
       <c r="C137" s="3">
         <v>50</v>
@@ -2664,46 +2664,46 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B138" s="3">
+      <c r="B138" s="4">
+        <v>56</v>
+      </c>
+      <c r="C138" s="3">
+        <v>50</v>
+      </c>
+      <c r="D138" s="3">
+        <v>70</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139" s="3">
         <v>57</v>
       </c>
-      <c r="C138" s="3">
-        <v>50</v>
-      </c>
-      <c r="D138" s="3">
-        <v>70</v>
-      </c>
-      <c r="E138" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B139" s="3">
-        <v>58</v>
-      </c>
       <c r="C139" s="3">
         <v>50</v>
       </c>
       <c r="D139" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="4">
-        <v>59</v>
+      <c r="B140" s="3">
+        <v>58</v>
       </c>
       <c r="C140" s="3">
         <v>50</v>
@@ -2711,13 +2711,16 @@
       <c r="D140" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E140" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="3">
-        <v>60</v>
+      <c r="B141" s="4">
+        <v>59</v>
       </c>
       <c r="C141" s="3">
         <v>50</v>
@@ -2726,48 +2729,63 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B142" s="3">
+        <v>60</v>
+      </c>
+      <c r="C142" s="3">
+        <v>50</v>
+      </c>
+      <c r="D142" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="3">
         <v>61</v>
       </c>
-      <c r="C142" s="3">
-        <v>50</v>
-      </c>
-      <c r="D142" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C143" s="3">
+        <v>50</v>
+      </c>
+      <c r="D143" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final ctc changes iteration 3
</commit_message>
<xml_diff>
--- a/Green Line Info.xlsx
+++ b/Green Line Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\1140-Integration-SWTrackController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433871E-5900-4E6C-AC7C-0FDC92A164C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{64DD429F-E320-45C6-AB13-F2972415AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302F893A-C4A4-491C-AF41-5DBF03532908}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="11660" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="45">
   <si>
     <t>Section</t>
   </si>
@@ -143,6 +143,9 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
+    <t>STATION; CENTRAL; UNDERDROUND</t>
+  </si>
+  <si>
     <t>STATION; INGLEWOOD; UNDERGROUND</t>
   </si>
   <si>
@@ -168,12 +171,6 @@
   </si>
   <si>
     <t>STATION;   CASTLE SHANNON</t>
-  </si>
-  <si>
-    <t>STATION; CENTRAL; UNDERGROUND</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -555,18 +552,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,43 +580,43 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="5">
-        <v>151</v>
-      </c>
-      <c r="C2" s="5">
-        <v>50</v>
-      </c>
-      <c r="D2" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3">
+        <v>60</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4">
-        <v>62</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="3">
+        <v>63</v>
       </c>
       <c r="C3" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3">
-        <v>60</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3">
         <v>100</v>
@@ -628,26 +625,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3">
-        <v>64</v>
+      <c r="B5" s="4">
+        <v>65</v>
       </c>
       <c r="C5" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D5" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4">
-        <v>65</v>
+      <c r="B6" s="3">
+        <v>66</v>
       </c>
       <c r="C6" s="3">
         <v>200</v>
@@ -655,30 +655,27 @@
       <c r="D6" s="3">
         <v>70</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D7" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
-        <v>67</v>
+      <c r="B8" s="4">
+        <v>68</v>
       </c>
       <c r="C8" s="3">
         <v>100</v>
@@ -687,26 +684,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4">
-        <v>68</v>
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>69</v>
       </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
@@ -715,12 +712,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3">
-        <v>70</v>
+      <c r="B11" s="4">
+        <v>71</v>
       </c>
       <c r="C11" s="3">
         <v>100</v>
@@ -729,12 +726,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
-        <v>71</v>
+      <c r="B12" s="3">
+        <v>72</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
@@ -743,12 +740,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3">
         <v>100</v>
@@ -756,13 +753,16 @@
       <c r="D13" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>73</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>74</v>
       </c>
       <c r="C14" s="3">
         <v>100</v>
@@ -770,16 +770,13 @@
       <c r="D14" s="3">
         <v>60</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
-        <v>74</v>
+      <c r="B15" s="3">
+        <v>75</v>
       </c>
       <c r="C15" s="3">
         <v>100</v>
@@ -788,12 +785,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" s="3">
         <v>100</v>
@@ -801,30 +798,33 @@
       <c r="D16" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C17" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D17" s="3">
-        <v>60</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>77</v>
+      <c r="B18" s="4">
+        <v>78</v>
       </c>
       <c r="C18" s="3">
         <v>300</v>
@@ -832,16 +832,13 @@
       <c r="D18" s="3">
         <v>70</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4">
-        <v>78</v>
+      <c r="B19" s="3">
+        <v>79</v>
       </c>
       <c r="C19" s="3">
         <v>300</v>
@@ -850,12 +847,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" s="3">
         <v>300</v>
@@ -864,12 +861,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" s="3">
         <v>300</v>
@@ -878,12 +875,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3">
-        <v>81</v>
+      <c r="B22" s="4">
+        <v>82</v>
       </c>
       <c r="C22" s="3">
         <v>300</v>
@@ -892,12 +889,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="4">
-        <v>82</v>
+      <c r="B23" s="3">
+        <v>83</v>
       </c>
       <c r="C23" s="3">
         <v>300</v>
@@ -906,12 +903,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C24" s="3">
         <v>300</v>
@@ -920,12 +917,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3">
         <v>300</v>
@@ -934,74 +931,74 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="3">
-        <v>85</v>
+        <v>17</v>
+      </c>
+      <c r="B26" s="4">
+        <v>86</v>
       </c>
       <c r="C26" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D26" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="4">
-        <v>86</v>
+      <c r="B27" s="3">
+        <v>87</v>
       </c>
       <c r="C27" s="3">
-        <v>100</v>
+        <v>86.6</v>
       </c>
       <c r="D27" s="3">
         <v>55</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="3">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="3">
-        <v>86.6</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B29" s="3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3">
         <v>55</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="3">
-        <v>89</v>
+      <c r="B30" s="4">
+        <v>90</v>
       </c>
       <c r="C30" s="3">
         <v>75</v>
@@ -1010,12 +1007,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4">
-        <v>90</v>
+      <c r="B31" s="3">
+        <v>91</v>
       </c>
       <c r="C31" s="3">
         <v>75</v>
@@ -1024,12 +1021,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="3">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" s="3">
         <v>75</v>
@@ -1038,12 +1035,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" s="3">
         <v>75</v>
@@ -1052,12 +1049,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="3">
-        <v>93</v>
+      <c r="B34" s="4">
+        <v>94</v>
       </c>
       <c r="C34" s="3">
         <v>75</v>
@@ -1066,12 +1063,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="4">
-        <v>94</v>
+      <c r="B35" s="3">
+        <v>95</v>
       </c>
       <c r="C35" s="3">
         <v>75</v>
@@ -1080,12 +1077,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="3">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="3">
         <v>75</v>
@@ -1093,13 +1090,16 @@
       <c r="D36" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C37" s="3">
         <v>75</v>
@@ -1107,16 +1107,13 @@
       <c r="D37" s="3">
         <v>55</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="3">
-        <v>97</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="4">
+        <v>98</v>
       </c>
       <c r="C38" s="3">
         <v>75</v>
@@ -1125,12 +1122,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="4">
-        <v>98</v>
+      <c r="B39" s="3">
+        <v>99</v>
       </c>
       <c r="C39" s="3">
         <v>75</v>
@@ -1139,12 +1136,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C40" s="3">
         <v>75</v>
@@ -1153,40 +1150,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="3">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="3">
-        <v>101</v>
+        <v>21</v>
+      </c>
+      <c r="B42" s="4">
+        <v>102</v>
       </c>
       <c r="C42" s="3">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="D42" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="4">
-        <v>102</v>
+      <c r="B43" s="3">
+        <v>103</v>
       </c>
       <c r="C43" s="3">
         <v>100</v>
@@ -1195,40 +1192,44 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="3">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C44" s="3">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D44" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B45" s="3">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C45" s="3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D45" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="5" t="str">
+        <f>E13</f>
+        <v>STATION; DORMONT</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="3">
-        <v>105</v>
+      <c r="B46" s="4">
+        <v>106</v>
       </c>
       <c r="C46" s="3">
         <v>100</v>
@@ -1236,45 +1237,41 @@
       <c r="D46" s="3">
         <v>60</v>
       </c>
-      <c r="E46" s="5" t="str">
-        <f>E14</f>
-        <v>STATION; DORMONT</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="4">
-        <v>106</v>
+      <c r="B47" s="3">
+        <v>107</v>
       </c>
       <c r="C47" s="3">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D47" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="3">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C48" s="3">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D48" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="3">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C49" s="3">
         <v>100</v>
@@ -1283,26 +1280,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="3">
-        <v>109</v>
+        <v>23</v>
+      </c>
+      <c r="B50" s="4">
+        <v>110</v>
       </c>
       <c r="C50" s="3">
         <v>100</v>
       </c>
       <c r="D50" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="4">
-        <v>110</v>
+      <c r="B51" s="3">
+        <v>111</v>
       </c>
       <c r="C51" s="3">
         <v>100</v>
@@ -1311,12 +1308,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C52" s="3">
         <v>100</v>
@@ -1325,12 +1322,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C53" s="3">
         <v>100</v>
@@ -1339,12 +1336,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="3">
-        <v>113</v>
+      <c r="B54" s="4">
+        <v>114</v>
       </c>
       <c r="C54" s="3">
         <v>100</v>
@@ -1352,13 +1349,17 @@
       <c r="D54" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="5" t="str">
+        <f>E5</f>
+        <v>STATION; GLENBURY</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="4">
-        <v>114</v>
+      <c r="B55" s="3">
+        <v>115</v>
       </c>
       <c r="C55" s="3">
         <v>100</v>
@@ -1366,17 +1367,13 @@
       <c r="D55" s="3">
         <v>70</v>
       </c>
-      <c r="E55" s="5" t="str">
-        <f>E6</f>
-        <v>STATION; GLENBURY</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="3">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C56" s="3">
         <v>100</v>
@@ -1385,26 +1382,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B57" s="3">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D57" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="3">
-        <v>117</v>
+      <c r="B58" s="4">
+        <v>118</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
@@ -1413,40 +1410,40 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="4">
-        <v>118</v>
+      <c r="B59" s="3">
+        <v>119</v>
       </c>
       <c r="C59" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D59" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="3">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D60" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="3">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C61" s="3">
         <v>50</v>
@@ -1455,26 +1452,29 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="3">
-        <v>121</v>
+        <v>25</v>
+      </c>
+      <c r="B62" s="4">
+        <v>122</v>
       </c>
       <c r="C62" s="3">
         <v>50</v>
       </c>
       <c r="D62" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="4">
-        <v>122</v>
+      <c r="B63" s="3">
+        <v>123</v>
       </c>
       <c r="C63" s="3">
         <v>50</v>
@@ -1482,16 +1482,17 @@
       <c r="D63" s="3">
         <v>70</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E63" s="5" t="str">
+        <f>E138</f>
+        <v>STATION; OVERBROOK; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B64" s="3">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C64" s="3">
         <v>50</v>
@@ -1499,17 +1500,16 @@
       <c r="D64" s="3">
         <v>70</v>
       </c>
-      <c r="E64" s="5" t="str">
-        <f>E139</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="3">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C65" s="3">
         <v>50</v>
@@ -1521,12 +1521,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="3">
-        <v>125</v>
+      <c r="B66" s="4">
+        <v>126</v>
       </c>
       <c r="C66" s="3">
         <v>50</v>
@@ -1538,12 +1538,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="4">
-        <v>126</v>
+      <c r="B67" s="3">
+        <v>127</v>
       </c>
       <c r="C67" s="3">
         <v>50</v>
@@ -1555,12 +1555,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="3">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C68" s="3">
         <v>50</v>
@@ -1572,12 +1572,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B69" s="3">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C69" s="3">
         <v>50</v>
@@ -1589,12 +1589,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="3">
-        <v>129</v>
+      <c r="B70" s="4">
+        <v>130</v>
       </c>
       <c r="C70" s="3">
         <v>50</v>
@@ -1606,12 +1606,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B71" s="4">
-        <v>130</v>
+      <c r="B71" s="3">
+        <v>131</v>
       </c>
       <c r="C71" s="3">
         <v>50</v>
@@ -1623,12 +1623,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="3">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C72" s="3">
         <v>50</v>
@@ -1636,16 +1636,17 @@
       <c r="D72" s="3">
         <v>70</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E72" s="5" t="str">
+        <f>E129</f>
+        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="3">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C73" s="3">
         <v>50</v>
@@ -1653,17 +1654,16 @@
       <c r="D73" s="3">
         <v>70</v>
       </c>
-      <c r="E73" s="5" t="str">
-        <f>E130</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E73" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" s="3">
-        <v>133</v>
+      <c r="B74" s="4">
+        <v>134</v>
       </c>
       <c r="C74" s="3">
         <v>50</v>
@@ -1675,12 +1675,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="4">
-        <v>134</v>
+      <c r="B75" s="3">
+        <v>135</v>
       </c>
       <c r="C75" s="3">
         <v>50</v>
@@ -1692,12 +1692,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B76" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C76" s="3">
         <v>50</v>
@@ -1709,12 +1709,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B77" s="3">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C77" s="3">
         <v>50</v>
@@ -1726,12 +1726,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="3">
-        <v>137</v>
+      <c r="B78" s="4">
+        <v>138</v>
       </c>
       <c r="C78" s="3">
         <v>50</v>
@@ -1743,12 +1743,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="4">
-        <v>138</v>
+      <c r="B79" s="3">
+        <v>139</v>
       </c>
       <c r="C79" s="3">
         <v>50</v>
@@ -1760,12 +1760,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B80" s="3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C80" s="3">
         <v>50</v>
@@ -1777,12 +1777,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B81" s="3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C81" s="3">
         <v>50</v>
@@ -1790,34 +1790,31 @@
       <c r="D81" s="3">
         <v>70</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E81" s="5" t="str">
+        <f>E120</f>
+        <v>STATION; CENTRAL; UNDERDROUND</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B82" s="3">
-        <v>141</v>
+        <v>3</v>
+      </c>
+      <c r="B82" s="4">
+        <v>1</v>
       </c>
       <c r="C82" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D82" s="3">
-        <v>70</v>
-      </c>
-      <c r="E82" s="5" t="str">
-        <f>E121</f>
-        <v>STATION; CENTRAL; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="4">
-        <v>1</v>
+      <c r="B83" s="3">
+        <v>2</v>
       </c>
       <c r="C83" s="3">
         <v>100</v>
@@ -1825,13 +1822,16 @@
       <c r="D83" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E83" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84" s="3">
         <v>100</v>
@@ -1839,16 +1839,13 @@
       <c r="D84" s="3">
         <v>55</v>
       </c>
-      <c r="E84" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" s="3">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B85" s="4">
+        <v>4</v>
       </c>
       <c r="C85" s="3">
         <v>100</v>
@@ -1857,12 +1854,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="4">
-        <v>4</v>
+      <c r="B86" s="3">
+        <v>5</v>
       </c>
       <c r="C86" s="3">
         <v>100</v>
@@ -1871,26 +1868,26 @@
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="3">
+        <v>6</v>
+      </c>
+      <c r="C87" s="3">
+        <v>100</v>
+      </c>
+      <c r="D87" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="3">
-        <v>100</v>
-      </c>
-      <c r="D87" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="3">
-        <v>6</v>
+      <c r="B88" s="4">
+        <v>7</v>
       </c>
       <c r="C88" s="3">
         <v>100</v>
@@ -1898,13 +1895,14 @@
       <c r="D88" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E88" s="5"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="4">
-        <v>7</v>
+      <c r="B89" s="3">
+        <v>8</v>
       </c>
       <c r="C89" s="3">
         <v>100</v>
@@ -1912,14 +1910,13 @@
       <c r="D89" s="3">
         <v>55</v>
       </c>
-      <c r="E89" s="5"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B90" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C90" s="3">
         <v>100</v>
@@ -1927,13 +1924,16 @@
       <c r="D90" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E90" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="3">
-        <v>9</v>
+      <c r="B91" s="4">
+        <v>10</v>
       </c>
       <c r="C91" s="3">
         <v>100</v>
@@ -1941,16 +1941,13 @@
       <c r="D91" s="3">
         <v>55</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="4">
-        <v>10</v>
+      <c r="B92" s="3">
+        <v>11</v>
       </c>
       <c r="C92" s="3">
         <v>100</v>
@@ -1959,12 +1956,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="3">
-        <v>11</v>
+      <c r="B93" s="4">
+        <v>12</v>
       </c>
       <c r="C93" s="3">
         <v>100</v>
@@ -1972,30 +1969,30 @@
       <c r="D93" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E93" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94" s="4">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B94" s="3">
+        <v>13</v>
       </c>
       <c r="C94" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D94" s="3">
-        <v>55</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C95" s="3">
         <v>150</v>
@@ -2004,12 +2001,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="3">
-        <v>14</v>
+      <c r="B96" s="4">
+        <v>15</v>
       </c>
       <c r="C96" s="3">
         <v>150</v>
@@ -2018,12 +2015,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="4">
-        <v>15</v>
+      <c r="B97" s="3">
+        <v>16</v>
       </c>
       <c r="C97" s="3">
         <v>150</v>
@@ -2031,30 +2028,30 @@
       <c r="D97" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E97" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="3">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B98" s="4">
+        <v>17</v>
       </c>
       <c r="C98" s="3">
         <v>150</v>
       </c>
       <c r="D98" s="3">
-        <v>70</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B99" s="4">
-        <v>17</v>
+      <c r="B99" s="3">
+        <v>18</v>
       </c>
       <c r="C99" s="3">
         <v>150</v>
@@ -2063,12 +2060,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C100" s="3">
         <v>150</v>
@@ -2077,12 +2074,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="3">
-        <v>19</v>
+      <c r="B101" s="4">
+        <v>20</v>
       </c>
       <c r="C101" s="3">
         <v>150</v>
@@ -2091,26 +2088,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B102" s="4">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B102" s="3">
+        <v>21</v>
       </c>
       <c r="C102" s="3">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D102" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="3">
-        <v>21</v>
+      <c r="B103" s="4">
+        <v>22</v>
       </c>
       <c r="C103" s="3">
         <v>300</v>
@@ -2118,13 +2115,16 @@
       <c r="D103" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E103" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="4">
-        <v>22</v>
+      <c r="B104" s="3">
+        <v>23</v>
       </c>
       <c r="C104" s="3">
         <v>300</v>
@@ -2132,16 +2132,13 @@
       <c r="D104" s="3">
         <v>70</v>
       </c>
-      <c r="E104" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C105" s="3">
         <v>300</v>
@@ -2150,54 +2147,54 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="3">
-        <v>24</v>
+      <c r="B106" s="4">
+        <v>25</v>
       </c>
       <c r="C106" s="3">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D106" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="4">
-        <v>25</v>
+      <c r="B107" s="3">
+        <v>26</v>
       </c>
       <c r="C107" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D107" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="3">
-        <v>26</v>
+      <c r="B108" s="4">
+        <v>27</v>
       </c>
       <c r="C108" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D108" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="4">
-        <v>27</v>
+      <c r="B109" s="3">
+        <v>28</v>
       </c>
       <c r="C109" s="3">
         <v>50</v>
@@ -2206,12 +2203,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B110" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C110" s="3">
         <v>50</v>
@@ -2219,13 +2216,16 @@
       <c r="D110" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E110" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B111" s="3">
-        <v>29</v>
+      <c r="B111" s="4">
+        <v>30</v>
       </c>
       <c r="C111" s="3">
         <v>50</v>
@@ -2233,16 +2233,13 @@
       <c r="D111" s="3">
         <v>70</v>
       </c>
-      <c r="E111" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B112" s="4">
-        <v>30</v>
+      <c r="B112" s="3">
+        <v>31</v>
       </c>
       <c r="C112" s="3">
         <v>50</v>
@@ -2250,13 +2247,16 @@
       <c r="D112" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E112" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B113" s="3">
-        <v>31</v>
+      <c r="B113" s="4">
+        <v>32</v>
       </c>
       <c r="C113" s="3">
         <v>50</v>
@@ -2264,17 +2264,14 @@
       <c r="D113" s="3">
         <v>70</v>
       </c>
-      <c r="E113" s="5" t="s">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B114" s="4">
-        <v>32</v>
-      </c>
       <c r="C114" s="3">
         <v>50</v>
       </c>
@@ -2282,12 +2279,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B115" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C115" s="3">
         <v>50</v>
@@ -2296,12 +2293,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="3">
-        <v>34</v>
+      <c r="B116" s="4">
+        <v>35</v>
       </c>
       <c r="C116" s="3">
         <v>50</v>
@@ -2310,12 +2307,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B117" s="4">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="B117" s="3">
+        <v>36</v>
       </c>
       <c r="C117" s="3">
         <v>50</v>
@@ -2323,13 +2320,16 @@
       <c r="D117" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E117" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B118" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C118" s="3">
         <v>50</v>
@@ -2341,12 +2341,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="3">
-        <v>37</v>
+      <c r="B119" s="4">
+        <v>38</v>
       </c>
       <c r="C119" s="3">
         <v>50</v>
@@ -2358,12 +2358,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="4">
-        <v>38</v>
+      <c r="B120" s="3">
+        <v>39</v>
       </c>
       <c r="C120" s="3">
         <v>50</v>
@@ -2371,16 +2371,16 @@
       <c r="D120" s="3">
         <v>70</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E120" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B121" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C121" s="3">
         <v>50</v>
@@ -2388,16 +2388,16 @@
       <c r="D121" s="3">
         <v>70</v>
       </c>
-      <c r="E121" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E121" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="3">
-        <v>40</v>
+      <c r="B122" s="4">
+        <v>41</v>
       </c>
       <c r="C122" s="3">
         <v>50</v>
@@ -2409,12 +2409,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="4">
-        <v>41</v>
+      <c r="B123" s="3">
+        <v>42</v>
       </c>
       <c r="C123" s="3">
         <v>50</v>
@@ -2426,12 +2426,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B124" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C124" s="3">
         <v>50</v>
@@ -2443,12 +2443,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="3">
-        <v>43</v>
+      <c r="B125" s="4">
+        <v>44</v>
       </c>
       <c r="C125" s="3">
         <v>50</v>
@@ -2460,12 +2460,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="4">
-        <v>44</v>
+      <c r="B126" s="3">
+        <v>45</v>
       </c>
       <c r="C126" s="3">
         <v>50</v>
@@ -2477,12 +2477,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B127" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C127" s="3">
         <v>50</v>
@@ -2494,12 +2494,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="3">
-        <v>46</v>
+      <c r="B128" s="4">
+        <v>47</v>
       </c>
       <c r="C128" s="3">
         <v>50</v>
@@ -2511,12 +2511,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="4">
-        <v>47</v>
+      <c r="B129" s="3">
+        <v>48</v>
       </c>
       <c r="C129" s="3">
         <v>50</v>
@@ -2524,16 +2524,16 @@
       <c r="D129" s="3">
         <v>70</v>
       </c>
-      <c r="E129" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E129" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B130" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C130" s="3">
         <v>50</v>
@@ -2541,16 +2541,16 @@
       <c r="D130" s="3">
         <v>70</v>
       </c>
-      <c r="E130" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E130" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="3">
-        <v>49</v>
+      <c r="B131" s="4">
+        <v>50</v>
       </c>
       <c r="C131" s="3">
         <v>50</v>
@@ -2562,12 +2562,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="4">
-        <v>50</v>
+      <c r="B132" s="3">
+        <v>51</v>
       </c>
       <c r="C132" s="3">
         <v>50</v>
@@ -2579,12 +2579,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B133" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C133" s="3">
         <v>50</v>
@@ -2596,12 +2596,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B134" s="3">
-        <v>52</v>
+      <c r="B134" s="4">
+        <v>53</v>
       </c>
       <c r="C134" s="3">
         <v>50</v>
@@ -2613,12 +2613,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B135" s="4">
-        <v>53</v>
+      <c r="B135" s="3">
+        <v>54</v>
       </c>
       <c r="C135" s="3">
         <v>50</v>
@@ -2630,12 +2630,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B136" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C136" s="3">
         <v>50</v>
@@ -2647,12 +2647,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B137" s="3">
-        <v>55</v>
+      <c r="B137" s="4">
+        <v>56</v>
       </c>
       <c r="C137" s="3">
         <v>50</v>
@@ -2664,12 +2664,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B138" s="4">
-        <v>56</v>
+      <c r="B138" s="3">
+        <v>57</v>
       </c>
       <c r="C138" s="3">
         <v>50</v>
@@ -2677,33 +2677,33 @@
       <c r="D138" s="3">
         <v>70</v>
       </c>
-      <c r="E138" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E138" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B139" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C139" s="3">
         <v>50</v>
       </c>
       <c r="D139" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="3">
-        <v>58</v>
+      <c r="B140" s="4">
+        <v>59</v>
       </c>
       <c r="C140" s="3">
         <v>50</v>
@@ -2711,16 +2711,13 @@
       <c r="D140" s="3">
         <v>60</v>
       </c>
-      <c r="E140" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="4">
-        <v>59</v>
+      <c r="B141" s="3">
+        <v>60</v>
       </c>
       <c r="C141" s="3">
         <v>50</v>
@@ -2729,12 +2726,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B142" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C142" s="3">
         <v>50</v>
@@ -2743,49 +2740,34 @@
         <v>60</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B143" s="3">
-        <v>61</v>
-      </c>
-      <c r="C143" s="3">
-        <v>50</v>
-      </c>
-      <c r="D143" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D151" s="3"/>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D152" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use this code but not anyone at the same time
</commit_message>
<xml_diff>
--- a/Green Line Info.xlsx
+++ b/Green Line Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\1140-Integration-SWTrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{64DD429F-E320-45C6-AB13-F2972415AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{302F893A-C4A4-491C-AF41-5DBF03532908}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433871E-5900-4E6C-AC7C-0FDC92A164C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="46">
   <si>
     <t>Section</t>
   </si>
@@ -143,9 +143,6 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; CENTRAL; UNDERDROUND</t>
-  </si>
-  <si>
     <t>STATION; INGLEWOOD; UNDERGROUND</t>
   </si>
   <si>
@@ -171,6 +168,12 @@
   </si>
   <si>
     <t>STATION;   CASTLE SHANNON</t>
+  </si>
+  <si>
+    <t>STATION; CENTRAL; UNDERGROUND</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -552,18 +555,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,43 +583,43 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5">
+        <v>151</v>
+      </c>
+      <c r="C2" s="5">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>62</v>
       </c>
-      <c r="C2" s="3">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3">
-        <v>60</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3">
-        <v>63</v>
-      </c>
       <c r="C3" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3">
         <v>100</v>
@@ -625,29 +628,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
-        <v>65</v>
+      <c r="B5" s="3">
+        <v>64</v>
       </c>
       <c r="C5" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3">
         <v>70</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3">
-        <v>66</v>
+      <c r="B6" s="4">
+        <v>65</v>
       </c>
       <c r="C6" s="3">
         <v>200</v>
@@ -655,55 +655,58 @@
       <c r="D6" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D7" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
         <v>68</v>
       </c>
-      <c r="C8" s="3">
-        <v>100</v>
-      </c>
-      <c r="D8" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>69</v>
-      </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
@@ -712,12 +715,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
-        <v>71</v>
+      <c r="B11" s="3">
+        <v>70</v>
       </c>
       <c r="C11" s="3">
         <v>100</v>
@@ -726,12 +729,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
-        <v>72</v>
+      <c r="B12" s="4">
+        <v>71</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
@@ -740,43 +743,43 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3">
+        <v>72</v>
+      </c>
+      <c r="C13" s="3">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
         <v>73</v>
       </c>
-      <c r="C13" s="3">
-        <v>100</v>
-      </c>
-      <c r="D13" s="3">
-        <v>60</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <v>74</v>
-      </c>
       <c r="C14" s="3">
         <v>100</v>
       </c>
       <c r="D14" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3">
-        <v>75</v>
+      <c r="B15" s="4">
+        <v>74</v>
       </c>
       <c r="C15" s="3">
         <v>100</v>
@@ -785,46 +788,43 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
         <v>76</v>
       </c>
-      <c r="C16" s="3">
-        <v>100</v>
-      </c>
-      <c r="D16" s="3">
-        <v>60</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C17" s="3">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <v>60</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <v>77</v>
-      </c>
-      <c r="C17" s="3">
-        <v>300</v>
-      </c>
-      <c r="D17" s="3">
-        <v>70</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <v>78</v>
+      <c r="B18" s="3">
+        <v>77</v>
       </c>
       <c r="C18" s="3">
         <v>300</v>
@@ -832,13 +832,16 @@
       <c r="D18" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3">
-        <v>79</v>
+      <c r="B19" s="4">
+        <v>78</v>
       </c>
       <c r="C19" s="3">
         <v>300</v>
@@ -847,12 +850,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3">
         <v>300</v>
@@ -861,12 +864,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3">
         <v>300</v>
@@ -875,12 +878,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4">
-        <v>82</v>
+      <c r="B22" s="3">
+        <v>81</v>
       </c>
       <c r="C22" s="3">
         <v>300</v>
@@ -889,12 +892,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="3">
-        <v>83</v>
+      <c r="B23" s="4">
+        <v>82</v>
       </c>
       <c r="C23" s="3">
         <v>300</v>
@@ -903,12 +906,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="3">
         <v>300</v>
@@ -917,12 +920,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="3">
         <v>300</v>
@@ -931,74 +934,74 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="4">
-        <v>86</v>
+        <v>16</v>
+      </c>
+      <c r="B26" s="3">
+        <v>85</v>
       </c>
       <c r="C26" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D26" s="3">
-        <v>55</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="3">
-        <v>87</v>
+      <c r="B27" s="4">
+        <v>86</v>
       </c>
       <c r="C27" s="3">
-        <v>86.6</v>
+        <v>100</v>
       </c>
       <c r="D27" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="3">
+        <v>87</v>
+      </c>
+      <c r="C28" s="3">
+        <v>86.6</v>
+      </c>
+      <c r="D28" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3">
         <v>88</v>
       </c>
-      <c r="C28" s="3">
-        <v>100</v>
-      </c>
-      <c r="D28" s="3">
-        <v>55</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="3">
-        <v>89</v>
-      </c>
       <c r="C29" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D29" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4">
-        <v>90</v>
+      <c r="B30" s="3">
+        <v>89</v>
       </c>
       <c r="C30" s="3">
         <v>75</v>
@@ -1007,12 +1010,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="3">
-        <v>91</v>
+      <c r="B31" s="4">
+        <v>90</v>
       </c>
       <c r="C31" s="3">
         <v>75</v>
@@ -1021,12 +1024,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="3">
         <v>75</v>
@@ -1035,12 +1038,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3">
         <v>75</v>
@@ -1049,12 +1052,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="4">
-        <v>94</v>
+      <c r="B34" s="3">
+        <v>93</v>
       </c>
       <c r="C34" s="3">
         <v>75</v>
@@ -1063,12 +1066,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="3">
-        <v>95</v>
+      <c r="B35" s="4">
+        <v>94</v>
       </c>
       <c r="C35" s="3">
         <v>75</v>
@@ -1077,12 +1080,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="3">
         <v>75</v>
@@ -1090,16 +1093,13 @@
       <c r="D36" s="3">
         <v>55</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="3">
         <v>75</v>
@@ -1107,13 +1107,16 @@
       <c r="D37" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="4">
-        <v>98</v>
+        <v>18</v>
+      </c>
+      <c r="B38" s="3">
+        <v>97</v>
       </c>
       <c r="C38" s="3">
         <v>75</v>
@@ -1122,12 +1125,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="3">
-        <v>99</v>
+      <c r="B39" s="4">
+        <v>98</v>
       </c>
       <c r="C39" s="3">
         <v>75</v>
@@ -1136,12 +1139,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="3">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="3">
         <v>75</v>
@@ -1150,40 +1153,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="3">
+        <v>100</v>
+      </c>
+      <c r="C41" s="3">
+        <v>75</v>
+      </c>
+      <c r="D41" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B42" s="3">
         <v>101</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C42" s="3">
         <v>15</v>
       </c>
-      <c r="D41" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="4">
-        <v>102</v>
-      </c>
-      <c r="C42" s="3">
-        <v>100</v>
-      </c>
       <c r="D42" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="3">
-        <v>103</v>
+      <c r="B43" s="4">
+        <v>102</v>
       </c>
       <c r="C43" s="3">
         <v>100</v>
@@ -1192,44 +1195,40 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="3">
+        <v>103</v>
+      </c>
+      <c r="C44" s="3">
+        <v>100</v>
+      </c>
+      <c r="D44" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="3">
         <v>104</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C45" s="3">
         <v>80</v>
       </c>
-      <c r="D44" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="3">
-        <v>105</v>
-      </c>
-      <c r="C45" s="3">
-        <v>100</v>
-      </c>
       <c r="D45" s="3">
         <v>60</v>
       </c>
-      <c r="E45" s="5" t="str">
-        <f>E13</f>
-        <v>STATION; DORMONT</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="4">
-        <v>106</v>
+      <c r="B46" s="3">
+        <v>105</v>
       </c>
       <c r="C46" s="3">
         <v>100</v>
@@ -1237,69 +1236,73 @@
       <c r="D46" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="5" t="str">
+        <f>E14</f>
+        <v>STATION; DORMONT</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="3">
-        <v>107</v>
+      <c r="B47" s="4">
+        <v>106</v>
       </c>
       <c r="C47" s="3">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D47" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="3">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C48" s="3">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D48" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="3">
+        <v>108</v>
+      </c>
+      <c r="C49" s="3">
+        <v>100</v>
+      </c>
+      <c r="D49" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="3">
         <v>109</v>
       </c>
-      <c r="C49" s="3">
-        <v>100</v>
-      </c>
-      <c r="D49" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="4">
-        <v>110</v>
-      </c>
       <c r="C50" s="3">
         <v>100</v>
       </c>
       <c r="D50" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="3">
-        <v>111</v>
+      <c r="B51" s="4">
+        <v>110</v>
       </c>
       <c r="C51" s="3">
         <v>100</v>
@@ -1308,12 +1311,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" s="3">
         <v>100</v>
@@ -1322,12 +1325,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="3">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C53" s="3">
         <v>100</v>
@@ -1336,12 +1339,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="4">
-        <v>114</v>
+      <c r="B54" s="3">
+        <v>113</v>
       </c>
       <c r="C54" s="3">
         <v>100</v>
@@ -1349,17 +1352,13 @@
       <c r="D54" s="3">
         <v>70</v>
       </c>
-      <c r="E54" s="5" t="str">
-        <f>E5</f>
-        <v>STATION; GLENBURY</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="3">
-        <v>115</v>
+      <c r="B55" s="4">
+        <v>114</v>
       </c>
       <c r="C55" s="3">
         <v>100</v>
@@ -1367,41 +1366,45 @@
       <c r="D55" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E55" s="5" t="str">
+        <f>E6</f>
+        <v>STATION; GLENBURY</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="3">
+        <v>115</v>
+      </c>
+      <c r="C56" s="3">
+        <v>100</v>
+      </c>
+      <c r="D56" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="3">
         <v>116</v>
       </c>
-      <c r="C56" s="3">
-        <v>100</v>
-      </c>
-      <c r="D56" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="3">
-        <v>117</v>
-      </c>
       <c r="C57" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D57" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="4">
-        <v>118</v>
+      <c r="B58" s="3">
+        <v>117</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
@@ -1410,71 +1413,68 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="3">
-        <v>119</v>
+      <c r="B59" s="4">
+        <v>118</v>
       </c>
       <c r="C59" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D59" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="3">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C60" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D60" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="3">
+        <v>120</v>
+      </c>
+      <c r="C61" s="3">
+        <v>50</v>
+      </c>
+      <c r="D61" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="3">
         <v>121</v>
       </c>
-      <c r="C61" s="3">
-        <v>50</v>
-      </c>
-      <c r="D61" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="4">
-        <v>122</v>
-      </c>
       <c r="C62" s="3">
         <v>50</v>
       </c>
       <c r="D62" s="3">
-        <v>70</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="3">
-        <v>123</v>
+      <c r="B63" s="4">
+        <v>122</v>
       </c>
       <c r="C63" s="3">
         <v>50</v>
@@ -1482,17 +1482,16 @@
       <c r="D63" s="3">
         <v>70</v>
       </c>
-      <c r="E63" s="5" t="str">
-        <f>E138</f>
-        <v>STATION; OVERBROOK; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E63" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B64" s="3">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" s="3">
         <v>50</v>
@@ -1500,16 +1499,17 @@
       <c r="D64" s="3">
         <v>70</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E64" s="5" t="str">
+        <f>E139</f>
+        <v>STATION; OVERBROOK; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="3">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="3">
         <v>50</v>
@@ -1521,12 +1521,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="4">
-        <v>126</v>
+      <c r="B66" s="3">
+        <v>125</v>
       </c>
       <c r="C66" s="3">
         <v>50</v>
@@ -1538,12 +1538,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="3">
-        <v>127</v>
+      <c r="B67" s="4">
+        <v>126</v>
       </c>
       <c r="C67" s="3">
         <v>50</v>
@@ -1555,12 +1555,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="3">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C68" s="3">
         <v>50</v>
@@ -1572,12 +1572,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B69" s="3">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C69" s="3">
         <v>50</v>
@@ -1589,12 +1589,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="4">
-        <v>130</v>
+      <c r="B70" s="3">
+        <v>129</v>
       </c>
       <c r="C70" s="3">
         <v>50</v>
@@ -1606,12 +1606,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B71" s="3">
-        <v>131</v>
+      <c r="B71" s="4">
+        <v>130</v>
       </c>
       <c r="C71" s="3">
         <v>50</v>
@@ -1623,12 +1623,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="3">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C72" s="3">
         <v>50</v>
@@ -1636,17 +1636,16 @@
       <c r="D72" s="3">
         <v>70</v>
       </c>
-      <c r="E72" s="5" t="str">
-        <f>E129</f>
-        <v>STATION; INGLEWOOD; UNDERGROUND</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E72" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C73" s="3">
         <v>50</v>
@@ -1654,16 +1653,17 @@
       <c r="D73" s="3">
         <v>70</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E73" s="5" t="str">
+        <f>E130</f>
+        <v>STATION; INGLEWOOD; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B74" s="4">
-        <v>134</v>
+      <c r="B74" s="3">
+        <v>133</v>
       </c>
       <c r="C74" s="3">
         <v>50</v>
@@ -1675,12 +1675,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="3">
-        <v>135</v>
+      <c r="B75" s="4">
+        <v>134</v>
       </c>
       <c r="C75" s="3">
         <v>50</v>
@@ -1692,12 +1692,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B76" s="3">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C76" s="3">
         <v>50</v>
@@ -1709,12 +1709,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B77" s="3">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C77" s="3">
         <v>50</v>
@@ -1726,12 +1726,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="4">
-        <v>138</v>
+      <c r="B78" s="3">
+        <v>137</v>
       </c>
       <c r="C78" s="3">
         <v>50</v>
@@ -1743,12 +1743,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="3">
-        <v>139</v>
+      <c r="B79" s="4">
+        <v>138</v>
       </c>
       <c r="C79" s="3">
         <v>50</v>
@@ -1760,12 +1760,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B80" s="3">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C80" s="3">
         <v>50</v>
@@ -1777,44 +1777,47 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B81" s="3">
+        <v>140</v>
+      </c>
+      <c r="C81" s="3">
+        <v>50</v>
+      </c>
+      <c r="D81" s="3">
+        <v>70</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="3">
         <v>141</v>
       </c>
-      <c r="C81" s="3">
-        <v>50</v>
-      </c>
-      <c r="D81" s="3">
-        <v>70</v>
-      </c>
-      <c r="E81" s="5" t="str">
-        <f>E120</f>
-        <v>STATION; CENTRAL; UNDERDROUND</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="4">
-        <v>1</v>
-      </c>
       <c r="C82" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D82" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="E82" s="5" t="str">
+        <f>E121</f>
+        <v>STATION; CENTRAL; UNDERGROUND</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="3">
-        <v>2</v>
+      <c r="B83" s="4">
+        <v>1</v>
       </c>
       <c r="C83" s="3">
         <v>100</v>
@@ -1822,30 +1825,30 @@
       <c r="D83" s="3">
         <v>55</v>
       </c>
-      <c r="E83" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="3">
+        <v>2</v>
+      </c>
+      <c r="C84" s="3">
+        <v>100</v>
+      </c>
+      <c r="D84" s="3">
+        <v>55</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="3">
-        <v>100</v>
-      </c>
-      <c r="D84" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="4">
-        <v>4</v>
+      <c r="B85" s="3">
+        <v>3</v>
       </c>
       <c r="C85" s="3">
         <v>100</v>
@@ -1854,12 +1857,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="3">
-        <v>5</v>
+      <c r="B86" s="4">
+        <v>4</v>
       </c>
       <c r="C86" s="3">
         <v>100</v>
@@ -1868,41 +1871,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B87" s="3">
+        <v>5</v>
+      </c>
+      <c r="C87" s="3">
+        <v>100</v>
+      </c>
+      <c r="D87" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="3">
         <v>6</v>
       </c>
-      <c r="C87" s="3">
-        <v>100</v>
-      </c>
-      <c r="D87" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="4">
-        <v>7</v>
-      </c>
       <c r="C88" s="3">
         <v>100</v>
       </c>
       <c r="D88" s="3">
         <v>55</v>
       </c>
-      <c r="E88" s="5"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="3">
-        <v>8</v>
+      <c r="B89" s="4">
+        <v>7</v>
       </c>
       <c r="C89" s="3">
         <v>100</v>
@@ -1910,13 +1912,14 @@
       <c r="D89" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E89" s="5"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B90" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90" s="3">
         <v>100</v>
@@ -1924,16 +1927,13 @@
       <c r="D90" s="3">
         <v>55</v>
       </c>
-      <c r="E90" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="4">
-        <v>10</v>
+      <c r="B91" s="3">
+        <v>9</v>
       </c>
       <c r="C91" s="3">
         <v>100</v>
@@ -1941,13 +1941,16 @@
       <c r="D91" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E91" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="3">
-        <v>11</v>
+      <c r="B92" s="4">
+        <v>10</v>
       </c>
       <c r="C92" s="3">
         <v>100</v>
@@ -1956,43 +1959,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93" s="3">
+        <v>11</v>
+      </c>
+      <c r="C93" s="3">
+        <v>100</v>
+      </c>
+      <c r="D93" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="4">
         <v>12</v>
       </c>
-      <c r="C93" s="3">
-        <v>100</v>
-      </c>
-      <c r="D93" s="3">
-        <v>55</v>
-      </c>
-      <c r="E93" s="3" t="s">
+      <c r="C94" s="3">
+        <v>100</v>
+      </c>
+      <c r="D94" s="3">
+        <v>55</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" s="3">
-        <v>13</v>
-      </c>
-      <c r="C94" s="3">
-        <v>150</v>
-      </c>
-      <c r="D94" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B95" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95" s="3">
         <v>150</v>
@@ -2001,12 +2004,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="4">
-        <v>15</v>
+      <c r="B96" s="3">
+        <v>14</v>
       </c>
       <c r="C96" s="3">
         <v>150</v>
@@ -2015,12 +2018,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="3">
-        <v>16</v>
+      <c r="B97" s="4">
+        <v>15</v>
       </c>
       <c r="C97" s="3">
         <v>150</v>
@@ -2028,30 +2031,30 @@
       <c r="D97" s="3">
         <v>70</v>
       </c>
-      <c r="E97" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="4">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="B98" s="3">
+        <v>16</v>
       </c>
       <c r="C98" s="3">
         <v>150</v>
       </c>
       <c r="D98" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B99" s="3">
-        <v>18</v>
+      <c r="B99" s="4">
+        <v>17</v>
       </c>
       <c r="C99" s="3">
         <v>150</v>
@@ -2060,12 +2063,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C100" s="3">
         <v>150</v>
@@ -2074,12 +2077,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B101" s="4">
-        <v>20</v>
+      <c r="B101" s="3">
+        <v>19</v>
       </c>
       <c r="C101" s="3">
         <v>150</v>
@@ -2088,26 +2091,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" s="3">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="B102" s="4">
+        <v>20</v>
       </c>
       <c r="C102" s="3">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D102" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="4">
-        <v>22</v>
+      <c r="B103" s="3">
+        <v>21</v>
       </c>
       <c r="C103" s="3">
         <v>300</v>
@@ -2115,16 +2118,13 @@
       <c r="D103" s="3">
         <v>70</v>
       </c>
-      <c r="E103" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="3">
-        <v>23</v>
+      <c r="B104" s="4">
+        <v>22</v>
       </c>
       <c r="C104" s="3">
         <v>300</v>
@@ -2132,13 +2132,16 @@
       <c r="D104" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E104" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B105" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C105" s="3">
         <v>300</v>
@@ -2147,99 +2150,99 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="4">
-        <v>25</v>
+      <c r="B106" s="3">
+        <v>24</v>
       </c>
       <c r="C106" s="3">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D106" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="3">
-        <v>26</v>
+      <c r="B107" s="4">
+        <v>25</v>
       </c>
       <c r="C107" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D107" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="4">
-        <v>27</v>
+      <c r="B108" s="3">
+        <v>26</v>
       </c>
       <c r="C108" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D108" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="4">
+        <v>27</v>
+      </c>
+      <c r="C109" s="3">
+        <v>50</v>
+      </c>
+      <c r="D109" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="3">
         <v>28</v>
       </c>
-      <c r="C109" s="3">
-        <v>50</v>
-      </c>
-      <c r="D109" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B110" s="3">
-        <v>29</v>
-      </c>
       <c r="C110" s="3">
         <v>50</v>
       </c>
       <c r="D110" s="3">
         <v>70</v>
       </c>
-      <c r="E110" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B111" s="4">
+      <c r="B111" s="3">
+        <v>29</v>
+      </c>
+      <c r="C111" s="3">
+        <v>50</v>
+      </c>
+      <c r="D111" s="3">
+        <v>70</v>
+      </c>
+      <c r="E111" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="3">
-        <v>50</v>
-      </c>
-      <c r="D111" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B112" s="3">
-        <v>31</v>
+      <c r="B112" s="4">
+        <v>30</v>
       </c>
       <c r="C112" s="3">
         <v>50</v>
@@ -2247,31 +2250,31 @@
       <c r="D112" s="3">
         <v>70</v>
       </c>
-      <c r="E112" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B113" s="4">
+      <c r="B113" s="3">
+        <v>31</v>
+      </c>
+      <c r="C113" s="3">
+        <v>50</v>
+      </c>
+      <c r="D113" s="3">
+        <v>70</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" s="4">
         <v>32</v>
       </c>
-      <c r="C113" s="3">
-        <v>50</v>
-      </c>
-      <c r="D113" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B114" s="3">
-        <v>33</v>
-      </c>
       <c r="C114" s="3">
         <v>50</v>
       </c>
@@ -2279,12 +2282,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B115" s="3">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C115" s="3">
         <v>50</v>
@@ -2293,43 +2296,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="4">
+      <c r="B116" s="3">
+        <v>34</v>
+      </c>
+      <c r="C116" s="3">
+        <v>50</v>
+      </c>
+      <c r="D116" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="4">
         <v>35</v>
       </c>
-      <c r="C116" s="3">
-        <v>50</v>
-      </c>
-      <c r="D116" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B117" s="3">
-        <v>36</v>
-      </c>
       <c r="C117" s="3">
         <v>50</v>
       </c>
       <c r="D117" s="3">
         <v>70</v>
       </c>
-      <c r="E117" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B118" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C118" s="3">
         <v>50</v>
@@ -2341,12 +2341,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="4">
-        <v>38</v>
+      <c r="B119" s="3">
+        <v>37</v>
       </c>
       <c r="C119" s="3">
         <v>50</v>
@@ -2358,12 +2358,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="3">
-        <v>39</v>
+      <c r="B120" s="4">
+        <v>38</v>
       </c>
       <c r="C120" s="3">
         <v>50</v>
@@ -2371,16 +2371,16 @@
       <c r="D120" s="3">
         <v>70</v>
       </c>
-      <c r="E120" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E120" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B121" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C121" s="3">
         <v>50</v>
@@ -2388,16 +2388,16 @@
       <c r="D121" s="3">
         <v>70</v>
       </c>
-      <c r="E121" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E121" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="4">
-        <v>41</v>
+      <c r="B122" s="3">
+        <v>40</v>
       </c>
       <c r="C122" s="3">
         <v>50</v>
@@ -2409,12 +2409,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="3">
-        <v>42</v>
+      <c r="B123" s="4">
+        <v>41</v>
       </c>
       <c r="C123" s="3">
         <v>50</v>
@@ -2426,12 +2426,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B124" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C124" s="3">
         <v>50</v>
@@ -2443,12 +2443,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="4">
-        <v>44</v>
+      <c r="B125" s="3">
+        <v>43</v>
       </c>
       <c r="C125" s="3">
         <v>50</v>
@@ -2460,12 +2460,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="3">
-        <v>45</v>
+      <c r="B126" s="4">
+        <v>44</v>
       </c>
       <c r="C126" s="3">
         <v>50</v>
@@ -2477,12 +2477,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B127" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C127" s="3">
         <v>50</v>
@@ -2494,12 +2494,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="4">
-        <v>47</v>
+      <c r="B128" s="3">
+        <v>46</v>
       </c>
       <c r="C128" s="3">
         <v>50</v>
@@ -2511,12 +2511,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="3">
-        <v>48</v>
+      <c r="B129" s="4">
+        <v>47</v>
       </c>
       <c r="C129" s="3">
         <v>50</v>
@@ -2524,16 +2524,16 @@
       <c r="D129" s="3">
         <v>70</v>
       </c>
-      <c r="E129" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E129" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B130" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C130" s="3">
         <v>50</v>
@@ -2541,16 +2541,16 @@
       <c r="D130" s="3">
         <v>70</v>
       </c>
-      <c r="E130" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E130" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="4">
-        <v>50</v>
+      <c r="B131" s="3">
+        <v>49</v>
       </c>
       <c r="C131" s="3">
         <v>50</v>
@@ -2562,12 +2562,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="3">
-        <v>51</v>
+      <c r="B132" s="4">
+        <v>50</v>
       </c>
       <c r="C132" s="3">
         <v>50</v>
@@ -2579,12 +2579,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B133" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C133" s="3">
         <v>50</v>
@@ -2596,12 +2596,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B134" s="4">
-        <v>53</v>
+      <c r="B134" s="3">
+        <v>52</v>
       </c>
       <c r="C134" s="3">
         <v>50</v>
@@ -2613,12 +2613,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B135" s="3">
-        <v>54</v>
+      <c r="B135" s="4">
+        <v>53</v>
       </c>
       <c r="C135" s="3">
         <v>50</v>
@@ -2630,12 +2630,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B136" s="3">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C136" s="3">
         <v>50</v>
@@ -2647,12 +2647,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B137" s="4">
-        <v>56</v>
+      <c r="B137" s="3">
+        <v>55</v>
       </c>
       <c r="C137" s="3">
         <v>50</v>
@@ -2664,46 +2664,46 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B138" s="3">
+      <c r="B138" s="4">
+        <v>56</v>
+      </c>
+      <c r="C138" s="3">
+        <v>50</v>
+      </c>
+      <c r="D138" s="3">
+        <v>70</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139" s="3">
         <v>57</v>
       </c>
-      <c r="C138" s="3">
-        <v>50</v>
-      </c>
-      <c r="D138" s="3">
-        <v>70</v>
-      </c>
-      <c r="E138" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B139" s="3">
-        <v>58</v>
-      </c>
       <c r="C139" s="3">
         <v>50</v>
       </c>
       <c r="D139" s="3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="4">
-        <v>59</v>
+      <c r="B140" s="3">
+        <v>58</v>
       </c>
       <c r="C140" s="3">
         <v>50</v>
@@ -2711,13 +2711,16 @@
       <c r="D140" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E140" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="3">
-        <v>60</v>
+      <c r="B141" s="4">
+        <v>59</v>
       </c>
       <c r="C141" s="3">
         <v>50</v>
@@ -2726,48 +2729,63 @@
         <v>60</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B142" s="3">
+        <v>60</v>
+      </c>
+      <c r="C142" s="3">
+        <v>50</v>
+      </c>
+      <c r="D142" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="3">
         <v>61</v>
       </c>
-      <c r="C142" s="3">
-        <v>50</v>
-      </c>
-      <c r="D142" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C143" s="3">
+        <v>50</v>
+      </c>
+      <c r="D143" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148" s="3"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D152" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>